<commit_message>
role check and message handleing are not completed
</commit_message>
<xml_diff>
--- a/uploads/Upload_Result.xlsx
+++ b/uploads/Upload_Result.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deepa\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anand\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7218A3F8-DEFE-42E8-86B0-BD5E4EF47AAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C60BE01-3D17-475E-839C-DC688C5CD0FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3330" yWindow="3330" windowWidth="23535" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -60,9 +60,6 @@
     <t>Admin</t>
   </si>
   <si>
-    <t>Ram</t>
-  </si>
-  <si>
     <t>K</t>
   </si>
   <si>
@@ -79,6 +76,9 @@
   </si>
   <si>
     <t>Phone missing, Last Name missing</t>
+  </si>
+  <si>
+    <t>Joe</t>
   </si>
 </sst>
 </file>
@@ -420,7 +420,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -452,7 +454,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -467,28 +469,26 @@
         <v>9</v>
       </c>
       <c r="E2" s="2"/>
-      <c r="F2" s="4">
-        <v>33101</v>
-      </c>
+      <c r="F2" s="4"/>
       <c r="G2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E3" s="2">
         <v>4512457889</v>
@@ -497,10 +497,10 @@
         <v>33397</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>